<commit_message>
First draft of final version of TP_PLL
</commit_message>
<xml_diff>
--- a/TP_PLL/Classeur1.xlsx
+++ b/TP_PLL/Classeur1.xlsx
@@ -1,15 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed\Documents\Ahmed\TSP\Cours\2A\Electronique-Numerique\TP_PLL\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B135850-0483-42B9-9DA8-4616ACF32BC9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -72,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,7 +114,1057 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="51000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="80000">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="93000"/>
+                      <a:satMod val="130000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="94000"/>
+                      <a:satMod val="135000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="16200000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="35000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.250153105861767E-2"/>
+                  <c:y val="-5.0462962962962961E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$A$18:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.9695</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0209000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1646999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3847</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5036999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6211000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.7629000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7890000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$B$18:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>163</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ADF5-4135-9426-EFCBD264C65E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="448497744"/>
+        <c:axId val="448501680"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="448497744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1.9"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>u_2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> (V)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="448501680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="448501680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="60"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx2"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Fréquence (kHz)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx2"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="448497744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFF0D9C4-9BAA-484D-83C5-80EE0D7E3F11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -156,7 +1210,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -188,9 +1242,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,6 +1294,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -397,16 +1487,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +1504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -428,60 +1518,63 @@
         <v>1.72</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>36</v>
       </c>
       <c r="E3">
         <v>220</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3">
+        <v>2.37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>252</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>324</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>360</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -489,7 +1582,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -503,7 +1596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>60</v>
       </c>
@@ -514,12 +1607,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
+        <v>1.9695</v>
+      </c>
+      <c r="B18">
         <v>73</v>
-      </c>
-      <c r="B18">
-        <v>1.9695</v>
       </c>
       <c r="D18">
         <v>73</v>
@@ -528,12 +1621,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
+        <v>2.0209000000000001</v>
+      </c>
+      <c r="B19">
         <v>80</v>
-      </c>
-      <c r="B19">
-        <v>2.0209000000000001</v>
       </c>
       <c r="D19">
         <v>80</v>
@@ -542,12 +1635,12 @@
         <v>2.0293999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
+        <v>2.1646999999999998</v>
+      </c>
+      <c r="B20">
         <v>100</v>
-      </c>
-      <c r="B20">
-        <v>2.1646999999999998</v>
       </c>
       <c r="D20">
         <v>100</v>
@@ -556,12 +1649,12 @@
         <v>2.1983000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
+        <v>2.3847</v>
+      </c>
+      <c r="B21">
         <v>120</v>
-      </c>
-      <c r="B21">
-        <v>2.3847</v>
       </c>
       <c r="D21">
         <v>120</v>
@@ -570,12 +1663,12 @@
         <v>2.3757000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
+        <v>2.5036999999999998</v>
+      </c>
+      <c r="B22">
         <v>128.80000000000001</v>
-      </c>
-      <c r="B22">
-        <v>2.5036999999999998</v>
       </c>
       <c r="D22">
         <v>128.80000000000001</v>
@@ -584,12 +1677,12 @@
         <v>2.4563999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
+        <v>2.6211000000000002</v>
+      </c>
+      <c r="B23">
         <v>140</v>
-      </c>
-      <c r="B23">
-        <v>2.6211000000000002</v>
       </c>
       <c r="D23">
         <v>140</v>
@@ -598,12 +1691,12 @@
         <v>2.5621999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
+        <v>2.7629000000000001</v>
+      </c>
+      <c r="B24">
         <v>160</v>
-      </c>
-      <c r="B24">
-        <v>2.7629000000000001</v>
       </c>
       <c r="D24">
         <v>160</v>
@@ -612,12 +1705,12 @@
         <v>2.7582</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
+        <v>2.7890000000000001</v>
+      </c>
+      <c r="B25">
         <v>163</v>
-      </c>
-      <c r="B25">
-        <v>2.7890000000000001</v>
       </c>
       <c r="D25">
         <v>163</v>
@@ -626,7 +1719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>180</v>
       </c>
@@ -637,12 +1730,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -653,7 +1746,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -664,7 +1757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>9</v>
       </c>
@@ -678,7 +1771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -686,7 +1779,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="4:8">
+    <row r="33" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
         <v>8</v>
       </c>
@@ -702,29 +1795,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>